<commit_message>
update on income data
</commit_message>
<xml_diff>
--- a/Group 17/files/Copy of bank.xlsx
+++ b/Group 17/files/Copy of bank.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Swarnim\Desktop\study\comp3850\PACE-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Swarnim\Desktop\study\comp3850\PACE-Project\Group 17\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BDDF112-8BC4-4A23-83F3-24C423E85F3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A639E8-9DEB-4FC4-93AE-027E77BF6A45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="425">
   <si>
     <t>DATE</t>
   </si>
@@ -1302,6 +1302,9 @@
   </si>
   <si>
     <t>CUST_MORE</t>
+  </si>
+  <si>
+    <t>High</t>
   </si>
 </sst>
 </file>
@@ -1724,8 +1727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1993,7 +1996,7 @@
         <v>95</v>
       </c>
       <c r="D5">
-        <v>49200</v>
+        <v>29200</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
@@ -2045,13 +2048,13 @@
         <v>1075358</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>424</v>
       </c>
       <c r="D6">
-        <v>80000</v>
+        <v>800000</v>
       </c>
       <c r="E6" t="s">
         <v>90</v>
@@ -2164,10 +2167,10 @@
         <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>424</v>
       </c>
       <c r="D8">
-        <v>47004</v>
+        <v>470004</v>
       </c>
       <c r="E8" t="s">
         <v>90</v>
@@ -2225,7 +2228,7 @@
         <v>95</v>
       </c>
       <c r="D9">
-        <v>48000</v>
+        <v>18000</v>
       </c>
       <c r="E9" t="s">
         <v>90</v>
@@ -2283,7 +2286,7 @@
         <v>95</v>
       </c>
       <c r="D10">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="E10" t="s">
         <v>90</v>
@@ -2396,7 +2399,7 @@
         <v>93</v>
       </c>
       <c r="C12" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D12">
         <v>72000</v>
@@ -2454,7 +2457,7 @@
         <v>93</v>
       </c>
       <c r="C13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D13">
         <v>75000</v>
@@ -2625,13 +2628,13 @@
         <v>1069057</v>
       </c>
       <c r="B16" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D16">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -2747,7 +2750,7 @@
         <v>95</v>
       </c>
       <c r="D18">
-        <v>42000</v>
+        <v>38000</v>
       </c>
       <c r="E18" t="s">
         <v>12</v>
@@ -2805,7 +2808,7 @@
         <v>96</v>
       </c>
       <c r="D19">
-        <v>110000</v>
+        <v>61000</v>
       </c>
       <c r="E19" t="s">
         <v>13</v>
@@ -2863,7 +2866,7 @@
         <v>95</v>
       </c>
       <c r="D20">
-        <v>84000</v>
+        <v>34000</v>
       </c>
       <c r="E20" t="s">
         <v>14</v>
@@ -2921,7 +2924,7 @@
         <v>95</v>
       </c>
       <c r="D21">
-        <v>77385</v>
+        <v>17385</v>
       </c>
       <c r="E21" t="s">
         <v>15</v>
@@ -2979,7 +2982,7 @@
         <v>95</v>
       </c>
       <c r="D22">
-        <v>43370</v>
+        <v>23370</v>
       </c>
       <c r="E22" t="s">
         <v>16</v>
@@ -3034,10 +3037,10 @@
         <v>92</v>
       </c>
       <c r="C23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D23">
-        <v>105000</v>
+        <v>10500</v>
       </c>
       <c r="E23" t="s">
         <v>17</v>
@@ -3092,7 +3095,7 @@
         <v>93</v>
       </c>
       <c r="C24" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D24">
         <v>50000</v>
@@ -3150,7 +3153,7 @@
         <v>92</v>
       </c>
       <c r="C25" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D25">
         <v>50000</v>
@@ -3208,7 +3211,7 @@
         <v>92</v>
       </c>
       <c r="C26" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D26">
         <v>76000</v>
@@ -3266,7 +3269,7 @@
         <v>94</v>
       </c>
       <c r="C27" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D27">
         <v>92000</v>
@@ -3327,7 +3330,7 @@
         <v>95</v>
       </c>
       <c r="D28">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="E28" t="s">
         <v>22</v>
@@ -3385,7 +3388,7 @@
         <v>95</v>
       </c>
       <c r="D29">
-        <v>50004</v>
+        <v>30004</v>
       </c>
       <c r="E29" t="s">
         <v>23</v>
@@ -3440,7 +3443,7 @@
         <v>94</v>
       </c>
       <c r="C30" t="s">
-        <v>96</v>
+        <v>424</v>
       </c>
       <c r="D30">
         <v>106000</v>
@@ -3614,7 +3617,7 @@
         <v>94</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D33">
         <v>75000</v>
@@ -3849,7 +3852,7 @@
         <v>95</v>
       </c>
       <c r="D37">
-        <v>41000</v>
+        <v>31000</v>
       </c>
       <c r="E37" t="s">
         <v>31</v>
@@ -3907,7 +3910,7 @@
         <v>95</v>
       </c>
       <c r="D38">
-        <v>55596</v>
+        <v>35596</v>
       </c>
       <c r="E38" t="s">
         <v>32</v>
@@ -3965,7 +3968,7 @@
         <v>95</v>
       </c>
       <c r="D39">
-        <v>45000</v>
+        <v>35000</v>
       </c>
       <c r="E39" t="s">
         <v>33</v>
@@ -4139,7 +4142,7 @@
         <v>95</v>
       </c>
       <c r="D42">
-        <v>68004</v>
+        <v>38004</v>
       </c>
       <c r="E42" t="s">
         <v>36</v>
@@ -4197,7 +4200,7 @@
         <v>95</v>
       </c>
       <c r="D43">
-        <v>62300</v>
+        <v>32300</v>
       </c>
       <c r="E43" t="s">
         <v>37</v>
@@ -4255,7 +4258,7 @@
         <v>95</v>
       </c>
       <c r="D44">
-        <v>65000</v>
+        <v>35000</v>
       </c>
       <c r="E44" t="s">
         <v>38</v>
@@ -4313,7 +4316,7 @@
         <v>95</v>
       </c>
       <c r="D45">
-        <v>55000</v>
+        <v>35000</v>
       </c>
       <c r="E45" t="s">
         <v>39</v>
@@ -4368,7 +4371,7 @@
         <v>94</v>
       </c>
       <c r="C46" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D46">
         <v>45600</v>
@@ -4426,7 +4429,7 @@
         <v>92</v>
       </c>
       <c r="C47" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D47">
         <v>80000</v>
@@ -4484,7 +4487,7 @@
         <v>94</v>
       </c>
       <c r="C48" t="s">
-        <v>95</v>
+        <v>424</v>
       </c>
       <c r="D48">
         <v>100000</v>
@@ -4603,7 +4606,7 @@
         <v>95</v>
       </c>
       <c r="D50">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="E50" t="s">
         <v>44</v>
@@ -4661,7 +4664,7 @@
         <v>95</v>
       </c>
       <c r="D51">
-        <v>70000</v>
+        <v>30000</v>
       </c>
       <c r="E51" t="s">
         <v>45</v>
@@ -4719,7 +4722,7 @@
         <v>95</v>
       </c>
       <c r="D52">
-        <v>80000</v>
+        <v>20000</v>
       </c>
       <c r="E52" t="s">
         <v>46</v>
@@ -4777,7 +4780,7 @@
         <v>96</v>
       </c>
       <c r="D53">
-        <v>110000</v>
+        <v>70000</v>
       </c>
       <c r="E53" t="s">
         <v>47</v>
@@ -4835,7 +4838,7 @@
         <v>95</v>
       </c>
       <c r="D54">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="E54" t="s">
         <v>48</v>
@@ -4890,7 +4893,7 @@
         <v>92</v>
       </c>
       <c r="C55" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D55">
         <v>50000</v>
@@ -4951,7 +4954,7 @@
         <v>95</v>
       </c>
       <c r="D56">
-        <v>46000</v>
+        <v>26000</v>
       </c>
       <c r="E56" t="s">
         <v>50</v>
@@ -5006,7 +5009,7 @@
         <v>92</v>
       </c>
       <c r="C57" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D57">
         <v>50000</v>
@@ -5064,7 +5067,7 @@
         <v>92</v>
       </c>
       <c r="C58" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D58">
         <v>81000</v>
@@ -5180,7 +5183,7 @@
         <v>92</v>
       </c>
       <c r="C60" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D60">
         <v>51400</v>
@@ -5357,7 +5360,7 @@
         <v>95</v>
       </c>
       <c r="D63">
-        <v>40000</v>
+        <v>39000</v>
       </c>
       <c r="E63" t="s">
         <v>57</v>
@@ -5415,7 +5418,7 @@
         <v>95</v>
       </c>
       <c r="D64">
-        <v>50000</v>
+        <v>39000</v>
       </c>
       <c r="E64" t="s">
         <v>58</v>
@@ -5470,7 +5473,7 @@
         <v>92</v>
       </c>
       <c r="C65" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D65">
         <v>62000</v>
@@ -5528,7 +5531,7 @@
         <v>92</v>
       </c>
       <c r="C66" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D66">
         <v>45996</v>
@@ -5586,7 +5589,7 @@
         <v>94</v>
       </c>
       <c r="C67" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D67">
         <v>55000</v>
@@ -5705,7 +5708,7 @@
         <v>95</v>
       </c>
       <c r="D69">
-        <v>44544</v>
+        <v>34544</v>
       </c>
       <c r="E69" t="s">
         <v>63</v>
@@ -5763,7 +5766,7 @@
         <v>95</v>
       </c>
       <c r="D70">
-        <v>75000</v>
+        <v>25000</v>
       </c>
       <c r="E70" t="s">
         <v>64</v>
@@ -5821,7 +5824,7 @@
         <v>95</v>
       </c>
       <c r="D71">
-        <v>61000</v>
+        <v>21000</v>
       </c>
       <c r="E71" t="s">
         <v>65</v>
@@ -5879,7 +5882,7 @@
         <v>95</v>
       </c>
       <c r="D72">
-        <v>44000</v>
+        <v>24000</v>
       </c>
       <c r="E72" t="s">
         <v>66</v>
@@ -5937,7 +5940,7 @@
         <v>95</v>
       </c>
       <c r="D73">
-        <v>75000</v>
+        <v>35000</v>
       </c>
       <c r="E73" t="s">
         <v>67</v>
@@ -6053,7 +6056,7 @@
         <v>95</v>
       </c>
       <c r="D75">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="E75" t="s">
         <v>69</v>
@@ -6108,7 +6111,7 @@
         <v>93</v>
       </c>
       <c r="C76" t="s">
-        <v>96</v>
+        <v>424</v>
       </c>
       <c r="D76">
         <v>150000</v>
@@ -6166,7 +6169,7 @@
         <v>92</v>
       </c>
       <c r="C77" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D77">
         <v>90000</v>
@@ -6224,7 +6227,7 @@
         <v>94</v>
       </c>
       <c r="C78" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D78">
         <v>48000</v>
@@ -6282,7 +6285,7 @@
         <v>92</v>
       </c>
       <c r="C79" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D79">
         <v>75000</v>
@@ -6340,7 +6343,7 @@
         <v>94</v>
       </c>
       <c r="C80" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D80">
         <v>52000</v>
@@ -6398,7 +6401,7 @@
         <v>94</v>
       </c>
       <c r="C81" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D81">
         <v>65000</v>
@@ -6456,7 +6459,7 @@
         <v>94</v>
       </c>
       <c r="C82" t="s">
-        <v>96</v>
+        <v>424</v>
       </c>
       <c r="D82">
         <v>150000</v>
@@ -6517,7 +6520,7 @@
         <v>95</v>
       </c>
       <c r="D83">
-        <v>68000</v>
+        <v>38000</v>
       </c>
       <c r="E83" t="s">
         <v>77</v>
@@ -6572,10 +6575,10 @@
         <v>92</v>
       </c>
       <c r="C84" t="s">
-        <v>95</v>
+        <v>424</v>
       </c>
       <c r="D84">
-        <v>42000</v>
+        <v>332000</v>
       </c>
       <c r="E84" t="s">
         <v>78</v>
@@ -6630,10 +6633,10 @@
         <v>92</v>
       </c>
       <c r="C85" t="s">
-        <v>95</v>
+        <v>424</v>
       </c>
       <c r="D85">
-        <v>53000</v>
+        <v>153000</v>
       </c>
       <c r="E85" t="s">
         <v>90</v>
@@ -6685,7 +6688,7 @@
         <v>1068744</v>
       </c>
       <c r="B86" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C86" t="s">
         <v>95</v>
@@ -6746,7 +6749,7 @@
         <v>92</v>
       </c>
       <c r="C87" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D87">
         <v>60000</v>
@@ -6862,10 +6865,10 @@
         <v>94</v>
       </c>
       <c r="C89" t="s">
-        <v>95</v>
+        <v>424</v>
       </c>
       <c r="D89">
-        <v>42000</v>
+        <v>242000</v>
       </c>
       <c r="E89" t="s">
         <v>90</v>
@@ -6923,7 +6926,7 @@
         <v>95</v>
       </c>
       <c r="D90">
-        <v>88365</v>
+        <v>28365</v>
       </c>
       <c r="E90" t="s">
         <v>79</v>
@@ -6981,7 +6984,7 @@
         <v>95</v>
       </c>
       <c r="D91">
-        <v>72000</v>
+        <v>22000</v>
       </c>
       <c r="E91" t="s">
         <v>80</v>
@@ -7039,7 +7042,7 @@
         <v>95</v>
       </c>
       <c r="D92">
-        <v>62000</v>
+        <v>22000</v>
       </c>
       <c r="E92" t="s">
         <v>81</v>
@@ -7097,7 +7100,7 @@
         <v>95</v>
       </c>
       <c r="D93">
-        <v>43680</v>
+        <v>33680</v>
       </c>
       <c r="E93" t="s">
         <v>82</v>
@@ -7152,7 +7155,7 @@
         <v>92</v>
       </c>
       <c r="C94" t="s">
-        <v>96</v>
+        <v>424</v>
       </c>
       <c r="D94">
         <v>120000</v>
@@ -7210,7 +7213,7 @@
         <v>92</v>
       </c>
       <c r="C95" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D95">
         <v>66000</v>
@@ -7326,7 +7329,7 @@
         <v>92</v>
       </c>
       <c r="C97" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D97">
         <v>85000</v>
@@ -7384,7 +7387,7 @@
         <v>94</v>
       </c>
       <c r="C98" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D98">
         <v>47800</v>
@@ -7445,7 +7448,7 @@
         <v>95</v>
       </c>
       <c r="D99">
-        <v>45000</v>
+        <v>35000</v>
       </c>
       <c r="E99" t="s">
         <v>88</v>
@@ -7497,10 +7500,10 @@
         <v>1068350</v>
       </c>
       <c r="B100" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C100" t="s">
-        <v>95</v>
+        <v>424</v>
       </c>
       <c r="D100">
         <v>83000</v>

</xml_diff>